<commit_message>
Added AngularJS to Project. Implemented data binding for patient info in the document.
</commit_message>
<xml_diff>
--- a/xlsxReader/sample knee patients.xlsx
+++ b/xlsxReader/sample knee patients.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="20" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t>DONAUDI</t>
   </si>
   <si>
-    <t>STEFANO</t>
-  </si>
-  <si>
     <t>Relax</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>Woof</t>
+  </si>
+  <si>
+    <t>STEPHANO</t>
   </si>
 </sst>
 </file>
@@ -319,7 +319,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -327,8 +327,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -343,26 +347,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,7 +703,7 @@
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -703,74 +711,74 @@
     <col min="1" max="1" width="4.1640625" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="10" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="10"/>
+    <col min="10" max="10" width="14" style="17" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="8"/>
     <col min="14" max="14" width="7.5" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" style="10" customWidth="1"/>
-    <col min="16" max="16" width="7.5" style="10" customWidth="1"/>
-    <col min="17" max="17" width="4.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="10" customWidth="1"/>
-    <col min="23" max="23" width="6.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.33203125" style="10" customWidth="1"/>
-    <col min="25" max="25" width="6" style="10" customWidth="1"/>
-    <col min="26" max="26" width="5.6640625" style="10" customWidth="1"/>
-    <col min="27" max="27" width="6.1640625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="8" customWidth="1"/>
+    <col min="16" max="16" width="7.5" style="8" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.33203125" style="8" customWidth="1"/>
+    <col min="25" max="25" width="6" style="8" customWidth="1"/>
+    <col min="26" max="26" width="5.6640625" style="8" customWidth="1"/>
+    <col min="27" max="27" width="6.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="11" customFormat="1" ht="13">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:27" s="9" customFormat="1" ht="13">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="10" t="s">
         <v>27</v>
       </c>
       <c r="R1" s="12" t="s">
@@ -785,45 +793,45 @@
       <c r="U1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="8" customFormat="1" ht="14" thickBot="1">
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
+    <row r="2" spans="1:27" s="6" customFormat="1" ht="14" thickBot="1">
+      <c r="J2" s="16"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:27" s="8" customFormat="1" ht="18" thickBot="1">
+    <row r="3" spans="1:27" s="6" customFormat="1" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,19 +847,19 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="7">
+        <v>57</v>
+      </c>
+      <c r="J3" s="3">
         <v>42323</v>
       </c>
       <c r="K3" s="2">
@@ -875,17 +883,17 @@
       <c r="Q3" s="5">
         <v>0</v>
       </c>
-      <c r="R3" s="6">
-        <v>42129</v>
-      </c>
-      <c r="S3" s="6">
-        <v>42129</v>
-      </c>
-      <c r="T3" s="6">
-        <v>42099</v>
-      </c>
-      <c r="U3" s="6">
-        <v>42099</v>
+      <c r="R3" s="14">
+        <v>5</v>
+      </c>
+      <c r="S3" s="14">
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3" s="14">
+        <v>4</v>
       </c>
       <c r="V3" s="5">
         <v>36.5</v>
@@ -906,7 +914,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="8" customFormat="1" ht="18" thickBot="1">
+    <row r="4" spans="1:27" s="6" customFormat="1" ht="18" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,20 +930,20 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="2">
-        <v>2012</v>
+      <c r="J4" s="3">
+        <v>41094</v>
       </c>
       <c r="K4" s="2">
         <v>5</v>
@@ -958,17 +966,17 @@
       <c r="Q4" s="5">
         <v>0</v>
       </c>
-      <c r="R4" s="6">
-        <v>42099</v>
-      </c>
-      <c r="S4" s="6">
-        <v>42099</v>
-      </c>
-      <c r="T4" s="6">
-        <v>42129</v>
-      </c>
-      <c r="U4" s="6">
-        <v>42129</v>
+      <c r="R4" s="14">
+        <v>4</v>
+      </c>
+      <c r="S4" s="14">
+        <v>4</v>
+      </c>
+      <c r="T4">
+        <v>5</v>
+      </c>
+      <c r="U4" s="14">
+        <v>5</v>
       </c>
       <c r="V4" s="5">
         <v>33</v>
@@ -989,7 +997,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="8" customFormat="1" ht="18" thickBot="1">
+    <row r="5" spans="1:27" s="6" customFormat="1" ht="18" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1013,7 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1015,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="3">
         <v>42349</v>
@@ -1041,17 +1049,17 @@
       <c r="Q5" s="5">
         <v>0</v>
       </c>
-      <c r="R5" s="6">
-        <v>42068</v>
-      </c>
-      <c r="S5" s="6">
-        <v>42068</v>
-      </c>
-      <c r="T5" s="6">
-        <v>42129</v>
-      </c>
-      <c r="U5" s="6">
-        <v>42129</v>
+      <c r="R5" s="14">
+        <v>3</v>
+      </c>
+      <c r="S5" s="14">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>5</v>
+      </c>
+      <c r="U5" s="14">
+        <v>5</v>
       </c>
       <c r="V5" s="5">
         <v>38.5</v>
@@ -1072,7 +1080,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="8" customFormat="1" ht="18" thickBot="1">
+    <row r="6" spans="1:27" s="6" customFormat="1" ht="18" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1096,7 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="1"/>
@@ -1098,7 +1106,7 @@
       <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="3">
         <v>42323</v>
       </c>
       <c r="K6" s="5"/>
@@ -1120,17 +1128,17 @@
       <c r="Q6" s="5">
         <v>0</v>
       </c>
-      <c r="R6" s="6">
-        <v>42099</v>
-      </c>
-      <c r="S6" s="6">
-        <v>42099</v>
-      </c>
-      <c r="T6" s="6">
-        <v>42099</v>
-      </c>
-      <c r="U6" s="6">
-        <v>42099</v>
+      <c r="R6" s="14">
+        <v>4</v>
+      </c>
+      <c r="S6" s="14">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6" s="14">
+        <v>4</v>
       </c>
       <c r="V6" s="5">
         <v>38</v>
@@ -1151,7 +1159,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="8" customFormat="1" ht="18" thickBot="1">
+    <row r="7" spans="1:27" s="6" customFormat="1" ht="18" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1159,7 +1167,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
@@ -1167,7 +1175,7 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="1"/>
@@ -1201,17 +1209,17 @@
       <c r="Q7" s="5">
         <v>5</v>
       </c>
-      <c r="R7" s="6">
-        <v>42129</v>
-      </c>
-      <c r="S7" s="6">
-        <v>42129</v>
-      </c>
-      <c r="T7" s="6">
-        <v>42099</v>
-      </c>
-      <c r="U7" s="6">
-        <v>42099</v>
+      <c r="R7" s="14">
+        <v>5</v>
+      </c>
+      <c r="S7" s="14">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7" s="14">
+        <v>4</v>
       </c>
       <c r="V7" s="5">
         <v>35.5</v>

</xml_diff>